<commit_message>
Hakediş Tanımlama Sayfası Tamamlandı.
</commit_message>
<xml_diff>
--- a/Infoline.WorkOfTime/Infoline.WorkOfTime.WebProject/Content/SampleExcels/BayiHakedisOrnekExcel.xlsx
+++ b/Infoline.WorkOfTime/Infoline.WorkOfTime.WebProject/Content/SampleExcels/BayiHakedisOrnekExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infoline\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infoline\source\repos\Infoline-Bilgi-Teknolojileri\WorkOfTime-Web-Server\Infoline.WorkOfTime\Infoline.WorkOfTime.WebProject\Content\SampleExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54EA32CE-A24D-4036-A21D-08D4174A5D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F662A05-44AC-428F-AA18-D4806E653F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E38EAEDC-7A77-4113-940F-E6AD1B7B0B85}"/>
+    <workbookView xWindow="32220" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{E38EAEDC-7A77-4113-940F-E6AD1B7B0B85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,18 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>Imei</t>
-  </si>
-  <si>
-    <t>Satış Tarihi</t>
-  </si>
-  <si>
-    <t>Bayi Kodu</t>
-  </si>
-  <si>
-    <t>Bayi Adı</t>
-  </si>
-  <si>
     <t>351670620223565</t>
   </si>
   <si>
@@ -101,6 +89,18 @@
   </si>
   <si>
     <t>NC İLETİŞİM-NURİ CERTEL</t>
+  </si>
+  <si>
+    <t>Imei**</t>
+  </si>
+  <si>
+    <t>Satış Tarihi**</t>
+  </si>
+  <si>
+    <t>Bayi Kodu**</t>
+  </si>
+  <si>
+    <t>Bayi Adı**</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,100 +510,100 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>44594</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>44594</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>44593</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>44594</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>44594</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>